<commit_message>
added powo id, ipni id and plant name id to matched and accepted wcvp species
</commit_message>
<xml_diff>
--- a/splists_out/83_Zotz_Epiphytes_TableS1_WCVP_CHANGES_2026-02-25.xlsx
+++ b/splists_out/83_Zotz_Epiphytes_TableS1_WCVP_CHANGES_2026-02-25.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:AC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -455,30 +455,50 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>wcvp_accepted_id</t>
+          <t>wcvp_matched_plant_name_id</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>wcvp_matched_ipni_id</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>wcvp_accepted_plant_name_id</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>wcvp_accepted_powo_id</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>wcvp_accepted_ipni_id</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
           <t>wcvp_accepted_name</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>wcvp_accepted_family</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>wcvp_accepted_author</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>wcvp_lifeform_description</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>origmatches</t>
         </is>
@@ -556,24 +576,42 @@
         </is>
       </c>
       <c r="T2">
+        <v>3145712</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>22222-2</t>
+        </is>
+      </c>
+      <c r="V2">
         <v>3267566</v>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>77233624-1</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>77233624-1</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
         <is>
           <t>Asplenium erosum var. erosum</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>Aspleniaceae</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>perennial</t>
         </is>
       </c>
-      <c r="Y2" t="b">
+      <c r="AC2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -644,29 +682,47 @@
         </is>
       </c>
       <c r="T3">
+        <v>26873</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>619752-1</t>
+        </is>
+      </c>
+      <c r="V3">
         <v>523840</v>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>77174194-1</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>77174194-1</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>Bulbophyllum pinelianum</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>Ormerod</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y3" t="b">
+      <c r="AC3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -742,29 +798,47 @@
         </is>
       </c>
       <c r="T4">
+        <v>374688</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>60447792-2</t>
+        </is>
+      </c>
+      <c r="V4">
         <v>122779</v>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>155188-2</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>155188-2</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
         <is>
           <t>Maxillaria neglecta</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>L.O.Williams</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
+      <c r="AB4" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y4" t="b">
+      <c r="AC4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -840,29 +914,47 @@
         </is>
       </c>
       <c r="T5">
+        <v>33016</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>621590-1</t>
+        </is>
+      </c>
+      <c r="V5">
         <v>122713</v>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>643592-1</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>643592-1</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
         <is>
           <t>Maxillaria lutescens</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
         <is>
           <t>Scheidw.</t>
         </is>
       </c>
-      <c r="X5" t="inlineStr">
+      <c r="AB5" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y5" t="b">
+      <c r="AC5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -938,29 +1030,47 @@
         </is>
       </c>
       <c r="T6">
+        <v>372364</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>77086359-1</t>
+        </is>
+      </c>
+      <c r="V6">
         <v>123064</v>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>155331-2</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>155331-2</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
         <is>
           <t>Maxillaria uncata</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
         <is>
           <t>Lindl.</t>
         </is>
       </c>
-      <c r="X6" t="inlineStr">
+      <c r="AB6" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y6" t="b">
+      <c r="AC6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1040,20 +1150,38 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
+          <t>30051767-2</t>
+        </is>
+      </c>
+      <c r="V7">
+        <v>40369</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>30051767-2</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>30051767-2</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
           <t>Chysis</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
         <is>
           <t>Lindl.</t>
         </is>
       </c>
-      <c r="Y7" t="b">
+      <c r="AC7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1124,29 +1252,47 @@
         </is>
       </c>
       <c r="T8">
+        <v>2730126</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>62654-2</t>
+        </is>
+      </c>
+      <c r="V8">
         <v>2995272</v>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>77139499-1</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>77139499-1</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
         <is>
           <t>Codonanthopsis crassifolia</t>
         </is>
       </c>
-      <c r="V8" t="inlineStr">
+      <c r="Z8" t="inlineStr">
         <is>
           <t>Gesneriaceae</t>
         </is>
       </c>
-      <c r="W8" t="inlineStr">
+      <c r="AA8" t="inlineStr">
         <is>
           <t>Chautems &amp; Mat.Perret</t>
         </is>
       </c>
-      <c r="X8" t="inlineStr">
+      <c r="AB8" t="inlineStr">
         <is>
           <t>scrambling epiphyte</t>
         </is>
       </c>
-      <c r="Y8" t="b">
+      <c r="AC8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1217,29 +1363,47 @@
         </is>
       </c>
       <c r="T9">
+        <v>2730150</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>378732-1</t>
+        </is>
+      </c>
+      <c r="V9">
         <v>2995274</v>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>77139504-1</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>77139504-1</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
         <is>
           <t>Codonanthopsis uleana</t>
         </is>
       </c>
-      <c r="V9" t="inlineStr">
+      <c r="Z9" t="inlineStr">
         <is>
           <t>Gesneriaceae</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr">
+      <c r="AA9" t="inlineStr">
         <is>
           <t>Chautems &amp; Mat.Perret</t>
         </is>
       </c>
-      <c r="X9" t="inlineStr">
+      <c r="AB9" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y9" t="b">
+      <c r="AC9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1315,24 +1479,42 @@
         </is>
       </c>
       <c r="T10">
+        <v>3143114</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>77076643-1</t>
+        </is>
+      </c>
+      <c r="V10">
         <v>3155614</v>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>257328-2</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>257328-2</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
         <is>
           <t>Trichomanes ekmanii</t>
         </is>
       </c>
-      <c r="V10" t="inlineStr">
+      <c r="Z10" t="inlineStr">
         <is>
           <t>Hymenophyllaceae</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr">
+      <c r="AA10" t="inlineStr">
         <is>
           <t>Wess.Boer</t>
         </is>
       </c>
-      <c r="Y10" t="b">
+      <c r="AC10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1408,24 +1590,42 @@
         </is>
       </c>
       <c r="T11">
+        <v>3143119</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>77076664-1</t>
+        </is>
+      </c>
+      <c r="V11">
         <v>3155628</v>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>257344-2</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>257344-2</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
         <is>
           <t>Trichomanes godmanii</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr">
+      <c r="Z11" t="inlineStr">
         <is>
           <t>Hymenophyllaceae</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr">
+      <c r="AA11" t="inlineStr">
         <is>
           <t>Hook. ex Baker</t>
         </is>
       </c>
-      <c r="Y11" t="b">
+      <c r="AC11" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1501,24 +1701,42 @@
         </is>
       </c>
       <c r="T12">
+        <v>3143124</v>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>77076644-1</t>
+        </is>
+      </c>
+      <c r="V12">
         <v>3155664</v>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>257368-2</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>257368-2</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
         <is>
           <t>Trichomanes kapplerianum</t>
         </is>
       </c>
-      <c r="V12" t="inlineStr">
+      <c r="Z12" t="inlineStr">
         <is>
           <t>Hymenophyllaceae</t>
         </is>
       </c>
-      <c r="W12" t="inlineStr">
+      <c r="AA12" t="inlineStr">
         <is>
           <t>J.W.Sturm</t>
         </is>
       </c>
-      <c r="Y12" t="b">
+      <c r="AC12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1594,24 +1812,42 @@
         </is>
       </c>
       <c r="T13">
+        <v>3143126</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>17085120-1</t>
+        </is>
+      </c>
+      <c r="V13">
         <v>3155669</v>
       </c>
-      <c r="U13" t="inlineStr">
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>17230180-1</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>17230180-1</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
         <is>
           <t>Trichomanes krausii</t>
         </is>
       </c>
-      <c r="V13" t="inlineStr">
+      <c r="Z13" t="inlineStr">
         <is>
           <t>Hymenophyllaceae</t>
         </is>
       </c>
-      <c r="W13" t="inlineStr">
+      <c r="AA13" t="inlineStr">
         <is>
           <t>Hook. &amp; Grev.</t>
         </is>
       </c>
-      <c r="Y13" t="b">
+      <c r="AC13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1687,24 +1923,42 @@
         </is>
       </c>
       <c r="T14">
+        <v>3143138</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>80065-2</t>
+        </is>
+      </c>
+      <c r="V14">
         <v>3155704</v>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>257400-2</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>257400-2</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
         <is>
           <t>Trichomanes ovale</t>
         </is>
       </c>
-      <c r="V14" t="inlineStr">
+      <c r="Z14" t="inlineStr">
         <is>
           <t>Hymenophyllaceae</t>
         </is>
       </c>
-      <c r="W14" t="inlineStr">
+      <c r="AA14" t="inlineStr">
         <is>
           <t>Wess.Boer</t>
         </is>
       </c>
-      <c r="Y14" t="b">
+      <c r="AC14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1780,24 +2034,42 @@
         </is>
       </c>
       <c r="T15">
+        <v>3143141</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>17085290-1</t>
+        </is>
+      </c>
+      <c r="V15">
         <v>3155712</v>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>17231840-1</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>17231840-1</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
         <is>
           <t>Trichomanes punctatum</t>
         </is>
       </c>
-      <c r="V15" t="inlineStr">
+      <c r="Z15" t="inlineStr">
         <is>
           <t>Hymenophyllaceae</t>
         </is>
       </c>
-      <c r="W15" t="inlineStr">
+      <c r="AA15" t="inlineStr">
         <is>
           <t>Poir.</t>
         </is>
       </c>
-      <c r="Y15" t="b">
+      <c r="AC15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1882,25 +2154,43 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
+          <t>17103700-1</t>
+        </is>
+      </c>
+      <c r="V16">
+        <v>3152151</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>17103700-1</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>17103700-1</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
           <t>Elaphoglossum herminieri</t>
         </is>
       </c>
-      <c r="V16" t="inlineStr">
+      <c r="Z16" t="inlineStr">
         <is>
           <t>Polypodiaceae</t>
         </is>
       </c>
-      <c r="W16" t="inlineStr">
+      <c r="AA16" t="inlineStr">
         <is>
           <t>T.Moore</t>
         </is>
       </c>
-      <c r="X16" t="inlineStr">
+      <c r="AB16" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y16" t="b">
+      <c r="AC16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1985,25 +2275,43 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
+          <t>632948-1</t>
+        </is>
+      </c>
+      <c r="V17">
+        <v>69800</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>632948-1</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>632948-1</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
           <t>Epidendrum umbelliferum</t>
         </is>
       </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W17" t="inlineStr">
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
         <is>
           <t>J.F.Gmel.</t>
         </is>
       </c>
-      <c r="X17" t="inlineStr">
+      <c r="AB17" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y17" t="b">
+      <c r="AC17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2079,29 +2387,47 @@
         </is>
       </c>
       <c r="T18">
+        <v>247367</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>1141992-2</t>
+        </is>
+      </c>
+      <c r="V18">
         <v>496825</v>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>77151715-1</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>77151715-1</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
         <is>
           <t>Guarianthe hennisiana</t>
         </is>
       </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W18" t="inlineStr">
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
         <is>
           <t>Van den Berg</t>
         </is>
       </c>
-      <c r="X18" t="inlineStr">
+      <c r="AB18" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y18" t="b">
+      <c r="AC18" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2177,29 +2503,47 @@
         </is>
       </c>
       <c r="T19">
+        <v>249004</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>20010501-1</t>
+        </is>
+      </c>
+      <c r="V19">
         <v>122449</v>
       </c>
-      <c r="U19" t="inlineStr">
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>643387-1</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>643387-1</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
         <is>
           <t>Maxillaria crassifolia</t>
         </is>
       </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W19" t="inlineStr">
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
         <is>
           <t>Rchb.f.</t>
         </is>
       </c>
-      <c r="X19" t="inlineStr">
+      <c r="AB19" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y19" t="b">
+      <c r="AC19" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2270,29 +2614,47 @@
         </is>
       </c>
       <c r="T20">
+        <v>115049</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>142889-2</t>
+        </is>
+      </c>
+      <c r="V20">
         <v>115048</v>
       </c>
-      <c r="U20" t="inlineStr">
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>641735-1</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>641735-1</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
         <is>
           <t>Lockhartia parthenoglossa</t>
         </is>
       </c>
-      <c r="V20" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W20" t="inlineStr">
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
         <is>
           <t>Rchb.f.</t>
         </is>
       </c>
-      <c r="X20" t="inlineStr">
+      <c r="AB20" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y20" t="b">
+      <c r="AC20" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2363,29 +2725,47 @@
         </is>
       </c>
       <c r="T21">
+        <v>2508288</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>153428-2</t>
+        </is>
+      </c>
+      <c r="V21">
         <v>2840332</v>
       </c>
-      <c r="U21" t="inlineStr">
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>118130-2</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>118130-2</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
         <is>
           <t>Hawkesiophyton ulei</t>
         </is>
       </c>
-      <c r="V21" t="inlineStr">
+      <c r="Z21" t="inlineStr">
         <is>
           <t>Solanaceae</t>
         </is>
       </c>
-      <c r="W21" t="inlineStr">
+      <c r="AA21" t="inlineStr">
         <is>
           <t>Hunz.</t>
         </is>
       </c>
-      <c r="X21" t="inlineStr">
+      <c r="AB21" t="inlineStr">
         <is>
           <t>climbing epiphyte</t>
         </is>
       </c>
-      <c r="Y21" t="b">
+      <c r="AC21" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2460,25 +2840,43 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
+          <t>323005-2</t>
+        </is>
+      </c>
+      <c r="V22">
+        <v>121529</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>323005-2</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>323005-2</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
           <t>Masdevallia livingstoneana</t>
         </is>
       </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W22" t="inlineStr">
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
         <is>
           <t>Roezl ex Rchb.f.</t>
         </is>
       </c>
-      <c r="X22" t="inlineStr">
+      <c r="AB22" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y22" t="b">
+      <c r="AC22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2553,25 +2951,43 @@
       </c>
       <c r="U23" t="inlineStr">
         <is>
+          <t>309952-2</t>
+        </is>
+      </c>
+      <c r="V23">
+        <v>122877</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>309952-2</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>309952-2</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
           <t>Maxillaria powellii</t>
         </is>
       </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W23" t="inlineStr">
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
         <is>
           <t>Schltr.</t>
         </is>
       </c>
-      <c r="X23" t="inlineStr">
+      <c r="AB23" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y23" t="b">
+      <c r="AC23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2647,29 +3063,47 @@
         </is>
       </c>
       <c r="T24">
+        <v>374874</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>60448161-2</t>
+        </is>
+      </c>
+      <c r="V24">
         <v>122277</v>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>318683-2</t>
+        </is>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>318683-2</t>
+        </is>
+      </c>
+      <c r="Y24" t="inlineStr">
         <is>
           <t>Maxillaria acervata</t>
         </is>
       </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W24" t="inlineStr">
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
         <is>
           <t>Rchb.f.</t>
         </is>
       </c>
-      <c r="X24" t="inlineStr">
+      <c r="AB24" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y24" t="b">
+      <c r="AC24" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2745,29 +3179,47 @@
         </is>
       </c>
       <c r="T25">
+        <v>374875</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>60448162-2</t>
+        </is>
+      </c>
+      <c r="V25">
         <v>122293</v>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>643250-1</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>643250-1</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
         <is>
           <t>Maxillaria alba</t>
         </is>
       </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W25" t="inlineStr">
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
         <is>
           <t>Lindl.</t>
         </is>
       </c>
-      <c r="X25" t="inlineStr">
+      <c r="AB25" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y25" t="b">
+      <c r="AC25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2843,29 +3295,47 @@
         </is>
       </c>
       <c r="T26">
+        <v>374855</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>60448261-2</t>
+        </is>
+      </c>
+      <c r="V26">
         <v>123081</v>
       </c>
-      <c r="U26" t="inlineStr">
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>30044409-2</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>30044409-2</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
         <is>
           <t>Maxillaria variabilis</t>
         </is>
       </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W26" t="inlineStr">
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA26" t="inlineStr">
         <is>
           <t>Bateman ex Lindl.</t>
         </is>
       </c>
-      <c r="X26" t="inlineStr">
+      <c r="AB26" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y26" t="b">
+      <c r="AC26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2951,29 +3421,47 @@
         </is>
       </c>
       <c r="T27">
+        <v>129572</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>163911-2</t>
+        </is>
+      </c>
+      <c r="V27">
         <v>491533</v>
       </c>
-      <c r="U27" t="inlineStr">
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>77140627-1</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>77140627-1</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
         <is>
           <t>Monstera adansonii subsp. laniata</t>
         </is>
       </c>
-      <c r="V27" t="inlineStr">
+      <c r="Z27" t="inlineStr">
         <is>
           <t>Araceae</t>
         </is>
       </c>
-      <c r="W27" t="inlineStr">
+      <c r="AA27" t="inlineStr">
         <is>
           <t>Mayo &amp; I.M.Andrade</t>
         </is>
       </c>
-      <c r="X27" t="inlineStr">
+      <c r="AB27" t="inlineStr">
         <is>
           <t>climber</t>
         </is>
       </c>
-      <c r="Y27" t="b">
+      <c r="AC27" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3048,25 +3536,43 @@
       </c>
       <c r="U28" t="inlineStr">
         <is>
+          <t>308776-2</t>
+        </is>
+      </c>
+      <c r="V28">
+        <v>130064</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>308776-2</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>308776-2</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
           <t>Mormodes powellii</t>
         </is>
       </c>
-      <c r="V28" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W28" t="inlineStr">
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
         <is>
           <t>Schltr.</t>
         </is>
       </c>
-      <c r="X28" t="inlineStr">
+      <c r="AB28" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y28" t="b">
+      <c r="AC28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3137,29 +3643,47 @@
         </is>
       </c>
       <c r="T29">
+        <v>139961</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>319316-2</t>
+        </is>
+      </c>
+      <c r="V29">
         <v>273887</v>
       </c>
-      <c r="U29" t="inlineStr">
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>77118514-1</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>77118514-1</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
         <is>
           <t>Trichocentrum lacerum</t>
         </is>
       </c>
-      <c r="V29" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W29" t="inlineStr">
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
         <is>
           <t>J.M.H.Shaw</t>
         </is>
       </c>
-      <c r="X29" t="inlineStr">
+      <c r="AB29" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y29" t="b">
+      <c r="AC29" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3230,29 +3754,47 @@
         </is>
       </c>
       <c r="T30">
+        <v>2555839</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>188992-2</t>
+        </is>
+      </c>
+      <c r="V30">
         <v>2558508</v>
       </c>
-      <c r="U30" t="inlineStr">
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>680010-1</t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>680010-1</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
         <is>
           <t>Peperomia tenuifolia</t>
         </is>
       </c>
-      <c r="V30" t="inlineStr">
+      <c r="Z30" t="inlineStr">
         <is>
           <t>Piperaceae</t>
         </is>
       </c>
-      <c r="W30" t="inlineStr">
+      <c r="AA30" t="inlineStr">
         <is>
           <t>C.DC.</t>
         </is>
       </c>
-      <c r="X30" t="inlineStr">
+      <c r="AB30" t="inlineStr">
         <is>
           <t>epiphyte or lithophyte</t>
         </is>
       </c>
-      <c r="Y30" t="b">
+      <c r="AC30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3327,20 +3869,38 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
+          <t>679124-1</t>
+        </is>
+      </c>
+      <c r="V31">
+        <v>2555657</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>679124-1</t>
+        </is>
+      </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>679124-1</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
           <t>Peperomia microstachya</t>
         </is>
       </c>
-      <c r="V31" t="inlineStr">
+      <c r="Z31" t="inlineStr">
         <is>
           <t>Piperaceae</t>
         </is>
       </c>
-      <c r="W31" t="inlineStr">
+      <c r="AA31" t="inlineStr">
         <is>
           <t>C.DC.</t>
         </is>
       </c>
-      <c r="Y31" t="b">
+      <c r="AC31" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3416,29 +3976,47 @@
         </is>
       </c>
       <c r="T32">
+        <v>3138143</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>1051848-2</t>
+        </is>
+      </c>
+      <c r="V32">
         <v>3139933</v>
       </c>
-      <c r="U32" t="inlineStr">
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>1090207-2</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>1090207-2</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
         <is>
           <t>Huperzia dichotoma</t>
         </is>
       </c>
-      <c r="V32" t="inlineStr">
+      <c r="Z32" t="inlineStr">
         <is>
           <t>Lycopodiaceae</t>
         </is>
       </c>
-      <c r="W32" t="inlineStr">
+      <c r="AA32" t="inlineStr">
         <is>
           <t>Trevis.</t>
         </is>
       </c>
-      <c r="X32" t="inlineStr">
+      <c r="AB32" t="inlineStr">
         <is>
           <t>epiphytic subshrub</t>
         </is>
       </c>
-      <c r="Y32" t="b">
+      <c r="AC32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3514,29 +4092,47 @@
         </is>
       </c>
       <c r="T33">
+        <v>374927</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>60448370-2</t>
+        </is>
+      </c>
+      <c r="V33">
         <v>122531</v>
       </c>
-      <c r="U33" t="inlineStr">
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>323052-2</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>323052-2</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
         <is>
           <t>Maxillaria friedrichsthalii</t>
         </is>
       </c>
-      <c r="V33" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W33" t="inlineStr">
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA33" t="inlineStr">
         <is>
           <t>Rchb.f.</t>
         </is>
       </c>
-      <c r="X33" t="inlineStr">
+      <c r="AB33" t="inlineStr">
         <is>
           <t>pseudobulbous epiphyte</t>
         </is>
       </c>
-      <c r="Y33" t="b">
+      <c r="AC33" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3611,25 +4207,43 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
+          <t>657888-1</t>
+        </is>
+      </c>
+      <c r="V34">
+        <v>192658</v>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>657888-1</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>657888-1</t>
+        </is>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
           <t>Sobralia fragrans</t>
         </is>
       </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W34" t="inlineStr">
+      <c r="Z34" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA34" t="inlineStr">
         <is>
           <t>Lindl.</t>
         </is>
       </c>
-      <c r="X34" t="inlineStr">
+      <c r="AB34" t="inlineStr">
         <is>
           <t>epiphyte or lithophyte</t>
         </is>
       </c>
-      <c r="Y34" t="b">
+      <c r="AC34" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3700,29 +4314,47 @@
         </is>
       </c>
       <c r="T35">
+        <v>192726</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>311532-2</t>
+        </is>
+      </c>
+      <c r="V35">
         <v>192693</v>
       </c>
-      <c r="U35" t="inlineStr">
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>657915-1</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>657915-1</t>
+        </is>
+      </c>
+      <c r="Y35" t="inlineStr">
         <is>
           <t>Sobralia macrophylla</t>
         </is>
       </c>
-      <c r="V35" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W35" t="inlineStr">
+      <c r="Z35" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA35" t="inlineStr">
         <is>
           <t>Rchb.f.</t>
         </is>
       </c>
-      <c r="X35" t="inlineStr">
+      <c r="AB35" t="inlineStr">
         <is>
           <t>perennial or epiphyte</t>
         </is>
       </c>
-      <c r="Y35" t="b">
+      <c r="AC35" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3793,29 +4425,47 @@
         </is>
       </c>
       <c r="T36">
+        <v>268545</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>124818-1</t>
+        </is>
+      </c>
+      <c r="V36">
         <v>522516</v>
       </c>
-      <c r="U36" t="inlineStr">
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>77158959-1</t>
+        </is>
+      </c>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>77158959-1</t>
+        </is>
+      </c>
+      <c r="Y36" t="inlineStr">
         <is>
           <t>Wallisia anceps</t>
         </is>
       </c>
-      <c r="V36" t="inlineStr">
+      <c r="Z36" t="inlineStr">
         <is>
           <t>Bromeliaceae</t>
         </is>
       </c>
-      <c r="W36" t="inlineStr">
+      <c r="AA36" t="inlineStr">
         <is>
           <t>Barfuss &amp; W.Till</t>
         </is>
       </c>
-      <c r="X36" t="inlineStr">
+      <c r="AB36" t="inlineStr">
         <is>
           <t>perennial</t>
         </is>
       </c>
-      <c r="Y36" t="b">
+      <c r="AC36" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3886,29 +4536,47 @@
         </is>
       </c>
       <c r="T37">
+        <v>269382</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>254063-2</t>
+        </is>
+      </c>
+      <c r="V37">
         <v>521251</v>
       </c>
-      <c r="U37" t="inlineStr">
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>77158945-1</t>
+        </is>
+      </c>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>77158945-1</t>
+        </is>
+      </c>
+      <c r="Y37" t="inlineStr">
         <is>
           <t>Lemeltonia monadelpha</t>
         </is>
       </c>
-      <c r="V37" t="inlineStr">
+      <c r="Z37" t="inlineStr">
         <is>
           <t>Bromeliaceae</t>
         </is>
       </c>
-      <c r="W37" t="inlineStr">
+      <c r="AA37" t="inlineStr">
         <is>
           <t>Barfuss &amp; W.Till</t>
         </is>
       </c>
-      <c r="X37" t="inlineStr">
+      <c r="AB37" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y37" t="b">
+      <c r="AC37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3984,24 +4652,42 @@
         </is>
       </c>
       <c r="T38">
+        <v>3027901</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>322215-2</t>
+        </is>
+      </c>
+      <c r="V38">
         <v>3021461</v>
       </c>
-      <c r="U38" t="inlineStr">
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>566733-1</t>
+        </is>
+      </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>566733-1</t>
+        </is>
+      </c>
+      <c r="Y38" t="inlineStr">
         <is>
           <t>Blakea parasitica</t>
         </is>
       </c>
-      <c r="V38" t="inlineStr">
+      <c r="Z38" t="inlineStr">
         <is>
           <t>Melastomataceae</t>
         </is>
       </c>
-      <c r="W38" t="inlineStr">
+      <c r="AA38" t="inlineStr">
         <is>
           <t>D.Don</t>
         </is>
       </c>
-      <c r="Y38" t="b">
+      <c r="AC38" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4072,29 +4758,47 @@
         </is>
       </c>
       <c r="T39">
+        <v>208714</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>660788-1</t>
+        </is>
+      </c>
+      <c r="V39">
         <v>521363</v>
       </c>
-      <c r="U39" t="inlineStr">
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>77155180-1</t>
+        </is>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>77155180-1</t>
+        </is>
+      </c>
+      <c r="Y39" t="inlineStr">
         <is>
           <t>Maxillaria egertoniana</t>
         </is>
       </c>
-      <c r="V39" t="inlineStr">
-        <is>
-          <t>Orchidaceae</t>
-        </is>
-      </c>
-      <c r="W39" t="inlineStr">
+      <c r="Z39" t="inlineStr">
+        <is>
+          <t>Orchidaceae</t>
+        </is>
+      </c>
+      <c r="AA39" t="inlineStr">
         <is>
           <t>Molinari</t>
         </is>
       </c>
-      <c r="X39" t="inlineStr">
+      <c r="AB39" t="inlineStr">
         <is>
           <t>pseudobulbous lithophyte</t>
         </is>
       </c>
-      <c r="Y39" t="b">
+      <c r="AC39" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4165,29 +4869,47 @@
         </is>
       </c>
       <c r="T40">
+        <v>271834</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>126151-1</t>
+        </is>
+      </c>
+      <c r="V40">
         <v>272293</v>
       </c>
-      <c r="U40" t="inlineStr">
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>991912-1</t>
+        </is>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>991912-1</t>
+        </is>
+      </c>
+      <c r="Y40" t="inlineStr">
         <is>
           <t>Werauhia gladioliflora</t>
         </is>
       </c>
-      <c r="V40" t="inlineStr">
+      <c r="Z40" t="inlineStr">
         <is>
           <t>Bromeliaceae</t>
         </is>
       </c>
-      <c r="W40" t="inlineStr">
+      <c r="AA40" t="inlineStr">
         <is>
           <t>J.R.Grant</t>
         </is>
       </c>
-      <c r="X40" t="inlineStr">
+      <c r="AB40" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y40" t="b">
+      <c r="AC40" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4258,29 +4980,47 @@
         </is>
       </c>
       <c r="T41">
+        <v>271866</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>126161-1</t>
+        </is>
+      </c>
+      <c r="V41">
         <v>269108</v>
       </c>
-      <c r="U41" t="inlineStr">
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>125215-1</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>125215-1</t>
+        </is>
+      </c>
+      <c r="Y41" t="inlineStr">
         <is>
           <t>Tillandsia heliconioides</t>
         </is>
       </c>
-      <c r="V41" t="inlineStr">
+      <c r="Z41" t="inlineStr">
         <is>
           <t>Bromeliaceae</t>
         </is>
       </c>
-      <c r="W41" t="inlineStr">
+      <c r="AA41" t="inlineStr">
         <is>
           <t>Kunth</t>
         </is>
       </c>
-      <c r="X41" t="inlineStr">
+      <c r="AB41" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y41" t="b">
+      <c r="AC41" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4351,29 +5091,47 @@
         </is>
       </c>
       <c r="T42">
+        <v>272084</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>267495-2</t>
+        </is>
+      </c>
+      <c r="V42">
         <v>272337</v>
       </c>
-      <c r="U42" t="inlineStr">
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>991922-1</t>
+        </is>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>991922-1</t>
+        </is>
+      </c>
+      <c r="Y42" t="inlineStr">
         <is>
           <t>Werauhia ringens</t>
         </is>
       </c>
-      <c r="V42" t="inlineStr">
+      <c r="Z42" t="inlineStr">
         <is>
           <t>Bromeliaceae</t>
         </is>
       </c>
-      <c r="W42" t="inlineStr">
+      <c r="AA42" t="inlineStr">
         <is>
           <t>J.R.Grant</t>
         </is>
       </c>
-      <c r="X42" t="inlineStr">
+      <c r="AB42" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y42" t="b">
+      <c r="AC42" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4444,29 +5202,47 @@
         </is>
       </c>
       <c r="T43">
+        <v>272103</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>126201-1</t>
+        </is>
+      </c>
+      <c r="V43">
         <v>272340</v>
       </c>
-      <c r="U43" t="inlineStr">
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>1099976-2</t>
+        </is>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>1099976-2</t>
+        </is>
+      </c>
+      <c r="Y43" t="inlineStr">
         <is>
           <t>Werauhia sanguinolenta</t>
         </is>
       </c>
-      <c r="V43" t="inlineStr">
+      <c r="Z43" t="inlineStr">
         <is>
           <t>Bromeliaceae</t>
         </is>
       </c>
-      <c r="W43" t="inlineStr">
+      <c r="AA43" t="inlineStr">
         <is>
           <t>J.R.Grant</t>
         </is>
       </c>
-      <c r="X43" t="inlineStr">
+      <c r="AB43" t="inlineStr">
         <is>
           <t>epiphyte</t>
         </is>
       </c>
-      <c r="Y43" t="b">
+      <c r="AC43" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>